<commit_message>
15-12-2016 -- 03:47 PM
</commit_message>
<xml_diff>
--- a/documents/unit-test-1.xlsx
+++ b/documents/unit-test-1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Test Cases</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Fill all mandatory fields but existing name, phone number, email and with file upload.</t>
+  </si>
+  <si>
+    <t>File Name : View Records.</t>
+  </si>
+  <si>
+    <t>Phone,Passcode,MasterKey</t>
   </si>
 </sst>
 </file>
@@ -275,6 +281,8 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -296,11 +304,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,32 +601,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -640,7 +646,7 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -708,20 +714,20 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -741,7 +747,7 @@
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -827,8 +833,111 @@
         <v>6</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="10"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="B4:C4"/>

</xml_diff>

<commit_message>
15-12-2016 --04:09 PM Excel file change
</commit_message>
<xml_diff>
--- a/documents/unit-test-1.xlsx
+++ b/documents/unit-test-1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Test Cases</t>
   </si>
@@ -135,6 +135,39 @@
   </si>
   <si>
     <t>Phone,Passcode,MasterKey</t>
+  </si>
+  <si>
+    <t>Fill all mandatory fields phone + name + email.</t>
+  </si>
+  <si>
+    <t>{"status":true,"private key":"70ee2fccf9b39a0ec806c9910a0204b9","error":0,"data":{"num_rows":1,"rows":[{"type_id":"1","p_id":"1","document_url":"14671099105577252166cf1e.docx","timestamp":"2016-06-28 15:31:50"}]}}</t>
+  </si>
+  <si>
+    <t>Fill all mandatory fields phone + email.</t>
+  </si>
+  <si>
+    <t>{"status":true,"private key":"e5f6e8d6b5164ef5ffa69645ef40154a","error":0,"data":{"num_rows":1,"rows":[{"type_id":"1","p_id":"1","document_url":"14671099105577252166cf1e.docx","timestamp":"2016-06-28 15:31:50"}]}}</t>
+  </si>
+  <si>
+    <t>Fill all mandatory fields phone + name.</t>
+  </si>
+  <si>
+    <t>{"status":true,"private key":"923ef495a37d3af4cb171e26996ecae0","error":0,"data":{"num_rows":1,"rows":[{"type_id":"1","p_id":"1","document_url":"14671099105577252166cf1e.docx","timestamp":"2016-06-28 15:31:50"}]}}</t>
+  </si>
+  <si>
+    <t>only name.</t>
+  </si>
+  <si>
+    <t>{"status":false,"private key":"","error":"You Should fill Phone or Email with Name.","data":[]}</t>
+  </si>
+  <si>
+    <t>Fill all mandatory fields but record not found.</t>
+  </si>
+  <si>
+    <t>{"status":false,"private key":"","error":"Name, Email &amp; Phone does not exists.","data":[]}</t>
+  </si>
+  <si>
+    <t>Matching combination must with all mandatory fields. Only name will not consider.</t>
   </si>
 </sst>
 </file>
@@ -283,6 +316,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,12 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,32 +634,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -714,20 +747,20 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -834,20 +867,20 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -876,10 +909,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -887,10 +920,10 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,10 +931,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,10 +942,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,18 +953,18 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="B47" t="s">
-        <v>19</v>
+      <c r="B46" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>